<commit_message>
Added in substance use
</commit_message>
<xml_diff>
--- a/metadata/2022/hwb_metadata_routing.xlsx
+++ b/metadata/2022/hwb_metadata_routing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scotsconnect-my.sharepoint.com/personal/victoria_dunn_gov_scot/Documents/Git Repos/HWB Rap Project/hwb-census/metadata/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="158" documentId="8_{4395AEFA-8934-42A6-B049-8F36C6F5ADA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02E61A18-8C67-4CCD-BA25-3F6380B20BA3}"/>
+  <xr:revisionPtr revIDLastSave="163" documentId="8_{4395AEFA-8934-42A6-B049-8F36C6F5ADA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15185554-1E8B-4C8D-8DD8-8399F127449D}"/>
   <bookViews>
-    <workbookView xWindow="-13860" yWindow="-16455" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{8E5FCDC9-F4FC-4B8E-8B14-A5DEBC9F3E68}"/>
+    <workbookView xWindow="28740" yWindow="-16470" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{8E5FCDC9-F4FC-4B8E-8B14-A5DEBC9F3E68}"/>
   </bookViews>
   <sheets>
     <sheet name="P5" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="S4" sheetId="7" r:id="rId7"/>
     <sheet name="S5" sheetId="8" r:id="rId8"/>
     <sheet name="S6" sheetId="9" r:id="rId9"/>
+    <sheet name="S4_SU" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="132">
   <si>
     <t>question</t>
   </si>
@@ -197,6 +198,249 @@
   </si>
   <si>
     <t>(sex_last_time_contraception_use != "Yes" &amp; sex_last_time_contraception_use != "Don't know") | (sex_contraception_type_1_condom == "Yes" | sex_contraception_type_1_implant == "Yes" | sex_contraception_type_1_coil_hormonal == "Yes" | sex_contraception_type_1_coil == "Yes" | sex_contraception_type_1_injection == "Yes" | sex_contraception_type_1_pill == "Yes" | sex_contraception_type_1_patch == "Yes" | sex_contraception_type_1_vring == "Yes")</t>
+  </si>
+  <si>
+    <t>drugs_use_frequency != "I take drugs at least once a week or more" &amp; drugs_use_frequency != "I take drugs once or twice a month"</t>
+  </si>
+  <si>
+    <t>drugs_use_last_year_type_other</t>
+  </si>
+  <si>
+    <t>drugs_use_last_year_type_tanning_pills</t>
+  </si>
+  <si>
+    <t>drugs_use_last_year_type_diet_pills</t>
+  </si>
+  <si>
+    <t>drugs_use_last_year_type_2c</t>
+  </si>
+  <si>
+    <t>drugs_use_last_year_type_lsd</t>
+  </si>
+  <si>
+    <t>drugs_use_last_year_type_synthetic_cannabinoids</t>
+  </si>
+  <si>
+    <t>drugs_use_last_year_type_ketamine</t>
+  </si>
+  <si>
+    <t>drugs_use_last_year_type_gear</t>
+  </si>
+  <si>
+    <t>drugs_use_last_year_type_cannabis</t>
+  </si>
+  <si>
+    <t>drugs_use_last_year_type_steroids</t>
+  </si>
+  <si>
+    <t>drugs_use_last_year_type_cocaine</t>
+  </si>
+  <si>
+    <t>drugs_use_last_year_type_mdma</t>
+  </si>
+  <si>
+    <t>drugs_use_last_year_type_methadone</t>
+  </si>
+  <si>
+    <t>drugs_use_last_year_type_mushrooms</t>
+  </si>
+  <si>
+    <t>drugs_use_last_year_type_heroin</t>
+  </si>
+  <si>
+    <t>drugs_use_last_year_type_benzos</t>
+  </si>
+  <si>
+    <t>drugs_use_last_year_type_cyroban</t>
+  </si>
+  <si>
+    <t>drugs_use_last_year_type_ecstasy</t>
+  </si>
+  <si>
+    <t>drugs_use_last_year_type_amphetamines</t>
+  </si>
+  <si>
+    <t>drugs_use_last_year_type_solvents</t>
+  </si>
+  <si>
+    <t>drugs_ever_taken != "Yes"</t>
+  </si>
+  <si>
+    <t>drugs_use_last_year</t>
+  </si>
+  <si>
+    <t>drugs_use_frequency</t>
+  </si>
+  <si>
+    <t>alcohol_ever_had_any != "Yes"</t>
+  </si>
+  <si>
+    <t>alcohol_last_provided_by</t>
+  </si>
+  <si>
+    <t>alcohol_drinking_allowed_at_home</t>
+  </si>
+  <si>
+    <t>alcohol_usual_drinking_location_elsewhere</t>
+  </si>
+  <si>
+    <t>alcohol_usual_drinking_location_outdoors</t>
+  </si>
+  <si>
+    <t>alcohol_usual_drinking_location_someones_home</t>
+  </si>
+  <si>
+    <t>alcohol_usual_drinking_location_home</t>
+  </si>
+  <si>
+    <t>alcohol_usual_drinking_location_party</t>
+  </si>
+  <si>
+    <t>alcohol_usual_drinking_location_club</t>
+  </si>
+  <si>
+    <t>alcohol_usual_drinking_location_pub</t>
+  </si>
+  <si>
+    <t>alcohol_usual_source</t>
+  </si>
+  <si>
+    <t>alcohol_frequency_getting_drunk</t>
+  </si>
+  <si>
+    <t>alcohol_frequency_type_other</t>
+  </si>
+  <si>
+    <t>alcohol_frequency_type_wine_fortified</t>
+  </si>
+  <si>
+    <t>alcohol_frequency_type_cider</t>
+  </si>
+  <si>
+    <t>alcohol_frequency_type_spirits</t>
+  </si>
+  <si>
+    <t>alcohol_frequency_type_alcopops</t>
+  </si>
+  <si>
+    <t>alcohol_frequency_type_wine</t>
+  </si>
+  <si>
+    <t>alcohol_frequency_type_beer</t>
+  </si>
+  <si>
+    <t>e_cigarettes_use_frequency != "I use e-cigarettes / vapes once a week or more" &amp; e_cigarettes_use_frequency != "I use e-cigarettes / vapes sometimes, but no more than once a month"</t>
+  </si>
+  <si>
+    <t>e_cigarettes_source_other</t>
+  </si>
+  <si>
+    <t>e_cigarettes_source_take_without_asking</t>
+  </si>
+  <si>
+    <t>e_cigarettes_source_parents_provide</t>
+  </si>
+  <si>
+    <t>e_cigarettes_source_siblings_provide</t>
+  </si>
+  <si>
+    <t>e_cigarettes_source_friends_provide</t>
+  </si>
+  <si>
+    <t>e_cigarettes_source_ask_adult_unknown</t>
+  </si>
+  <si>
+    <t>e_cigarettes_source_ask_adult_known</t>
+  </si>
+  <si>
+    <t>e_cigarettes_source_ask_minor_known</t>
+  </si>
+  <si>
+    <t>e_cigarettes_source_someone_else</t>
+  </si>
+  <si>
+    <t>e_cigarettes_source_friends_relatives</t>
+  </si>
+  <si>
+    <t>e_cigarettes_source_internet</t>
+  </si>
+  <si>
+    <t>e_cigarettes_source_street_market</t>
+  </si>
+  <si>
+    <t>e_cigarettes_source_hop_other</t>
+  </si>
+  <si>
+    <t>e_cigarettes_source_van</t>
+  </si>
+  <si>
+    <t>e_cigarettes_source_garage_shop</t>
+  </si>
+  <si>
+    <t>e_cigarettes_source_newsagent</t>
+  </si>
+  <si>
+    <t>e_cigarettes_source_supermarket</t>
+  </si>
+  <si>
+    <t>cigarettes_smoking_status != "I usually smoke more than six cigarettes a week" &amp; cigarettes_smoking_status != "I usually smoke between one and six cigarettes a week" &amp; cigarettes_smoking_status != "I sometimes smoke cigarettes now but I don't smoke as many as one a week"</t>
+  </si>
+  <si>
+    <t>cigarettes_daily_number</t>
+  </si>
+  <si>
+    <t>cigarettes_attempts_buying</t>
+  </si>
+  <si>
+    <t>cigarettes_source_other</t>
+  </si>
+  <si>
+    <t>cigarettes_source_take_without_asking</t>
+  </si>
+  <si>
+    <t>cigarettes_source_parents_provide</t>
+  </si>
+  <si>
+    <t>cigarettes_source_siblings_provide</t>
+  </si>
+  <si>
+    <t>cigarettes_source_friends_provide</t>
+  </si>
+  <si>
+    <t>cigarettes_source_ask_adult_unknown</t>
+  </si>
+  <si>
+    <t>cigarettes_source_ask_adult_known</t>
+  </si>
+  <si>
+    <t>cigarettes_source_ask_minor_known</t>
+  </si>
+  <si>
+    <t>cigarettes_source_someone_else</t>
+  </si>
+  <si>
+    <t>cigarettes_source_friends_relatives</t>
+  </si>
+  <si>
+    <t>cigarettes_source_internet</t>
+  </si>
+  <si>
+    <t>cigarettes_source_street_market</t>
+  </si>
+  <si>
+    <t>cigarettes_source_hop_other</t>
+  </si>
+  <si>
+    <t>cigarettes_source_van</t>
+  </si>
+  <si>
+    <t>cigarettes_source_garage_shop</t>
+  </si>
+  <si>
+    <t>cigarettes_source_newsagent</t>
+  </si>
+  <si>
+    <t>cigarettes_source_supermarket</t>
   </si>
 </sst>
 </file>
@@ -232,9 +476,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -250,10 +493,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -674,6 +913,646 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ECEC06D-D7CF-47FF-A850-82AE6DBB06DE}">
+  <dimension ref="A1:B78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B20" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>110</v>
+      </c>
+      <c r="B22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>104</v>
+      </c>
+      <c r="B28" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>98</v>
+      </c>
+      <c r="B34" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>86</v>
+      </c>
+      <c r="B45" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>84</v>
+      </c>
+      <c r="B47" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>82</v>
+      </c>
+      <c r="B49" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>81</v>
+      </c>
+      <c r="B50" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>79</v>
+      </c>
+      <c r="B52" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>78</v>
+      </c>
+      <c r="B53" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>77</v>
+      </c>
+      <c r="B54" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>74</v>
+      </c>
+      <c r="B56" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>73</v>
+      </c>
+      <c r="B57" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>71</v>
+      </c>
+      <c r="B59" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>70</v>
+      </c>
+      <c r="B60" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>69</v>
+      </c>
+      <c r="B61" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>63</v>
+      </c>
+      <c r="B67" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>62</v>
+      </c>
+      <c r="B68" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>61</v>
+      </c>
+      <c r="B69" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>60</v>
+      </c>
+      <c r="B70" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>59</v>
+      </c>
+      <c r="B71" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>58</v>
+      </c>
+      <c r="B72" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>57</v>
+      </c>
+      <c r="B73" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>56</v>
+      </c>
+      <c r="B74" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>55</v>
+      </c>
+      <c r="B75" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>54</v>
+      </c>
+      <c r="B76" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>53</v>
+      </c>
+      <c r="B77" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>52</v>
+      </c>
+      <c r="B78" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F2E4EF3-626E-4910-80BC-4F3EDE8A88BE}">
   <dimension ref="A1:B13"/>
@@ -1325,7 +2204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4352FD0-16B2-4C5D-BEB5-4817E4EFB123}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1485,11 +2364,11 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1525,11 +2404,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1734,10 +2613,10 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1774,10 +2653,10 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1982,10 +2861,10 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2022,10 +2901,10 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>